<commit_message>
Updated 2025 show winners
</commit_message>
<xml_diff>
--- a/public/2025_stea_show_winners.xlsx
+++ b/public/2025_stea_show_winners.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diamo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diamo\Desktop\STEA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82A1C0E6-AAAE-41CD-88E9-E70FA115F206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1D690E-42E8-4A28-8833-73CA8F596234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{FB16AFC0-14EA-4179-B1B4-9B9A45EB60A9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="136">
   <si>
     <t>DIVISION</t>
   </si>
@@ -430,6 +430,9 @@
   </si>
   <si>
     <t>5th</t>
+  </si>
+  <si>
+    <t>WILD ROSE</t>
   </si>
 </sst>
 </file>
@@ -838,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FA7F129-83AB-4817-AA69-4048428C71E8}">
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -1636,16 +1639,16 @@
         <v>20</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F43" s="2">
-        <v>6</v>
+        <v>7.5</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>8</v>
@@ -1656,67 +1659,64 @@
         <v>20</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F44" s="2">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F45" s="2">
+        <v>2</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F46" s="2">
-        <v>19</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>7</v>
@@ -1729,23 +1729,26 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="B48" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F48" s="2">
-        <v>10.5</v>
+        <v>19</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
@@ -1753,16 +1756,16 @@
         <v>22</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F49" s="2">
-        <v>8</v>
+        <v>10.5</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>8</v>
@@ -1773,16 +1776,16 @@
         <v>22</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F50" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>8</v>
@@ -1793,16 +1796,16 @@
         <v>22</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="F51" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>8</v>
@@ -1813,68 +1816,68 @@
         <v>22</v>
       </c>
       <c r="C52" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F52" s="2">
+        <v>5</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B53" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D53" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="E53" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F52" s="2">
+      <c r="F53" s="2">
         <v>3</v>
       </c>
-      <c r="G52" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
+      <c r="G53" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" s="2" t="s">
+      <c r="B55" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D55" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F54" s="2">
+      <c r="F55" s="2">
         <v>37</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B55" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F55" s="2">
-        <v>18</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>8</v>
@@ -1885,16 +1888,16 @@
         <v>5</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="F56" s="2">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>8</v>
@@ -1905,19 +1908,19 @@
         <v>5</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F57" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
@@ -1925,10 +1928,10 @@
         <v>5</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>31</v>
@@ -1945,19 +1948,19 @@
         <v>5</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="F59" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
@@ -1965,68 +1968,68 @@
         <v>5</v>
       </c>
       <c r="C60" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F60" s="2">
+        <v>4</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B61" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D61" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="E61" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F60" s="2">
+      <c r="F61" s="2">
         <v>2</v>
       </c>
-      <c r="G60" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
+      <c r="G61" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A62" s="2" t="s">
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F62" s="2">
-        <v>9</v>
-      </c>
-      <c r="G62" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B63" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F63" s="2">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>8</v>
@@ -2037,68 +2040,68 @@
         <v>20</v>
       </c>
       <c r="C64" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F64" s="2">
+        <v>5</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B65" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D65" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="E65" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F64" s="2">
+      <c r="F65" s="2">
         <v>2</v>
       </c>
-      <c r="G64" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
+      <c r="G65" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A66" s="2" t="s">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A67" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C66" s="2" t="s">
+      <c r="B67" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="D67" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E66" s="2" t="s">
+      <c r="E67" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F66" s="2">
+      <c r="F67" s="2">
         <v>21</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B67" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F67" s="2">
-        <v>18</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>8</v>
@@ -2109,16 +2112,16 @@
         <v>22</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>131</v>
+        <v>29</v>
       </c>
       <c r="F68" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>8</v>
@@ -2129,16 +2132,16 @@
         <v>22</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>16</v>
+        <v>131</v>
       </c>
       <c r="F69" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>8</v>
@@ -2149,19 +2152,19 @@
         <v>22</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="F70" s="2">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
@@ -2169,89 +2172,89 @@
         <v>22</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="F71" s="2">
         <v>12</v>
       </c>
       <c r="G71" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B72" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F72" s="2">
+        <v>12</v>
+      </c>
+      <c r="G72" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A72" s="4"/>
-      <c r="B72" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C72" s="2" t="s">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A73" s="4"/>
+      <c r="B73" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="D73" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="E73" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F72" s="2">
+      <c r="F73" s="2">
         <v>10</v>
       </c>
-      <c r="G72" s="2" t="s">
+      <c r="G73" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
-      <c r="G73" s="3"/>
-    </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A74" s="2" t="s">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A75" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C74" s="2" t="s">
+      <c r="B75" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D75" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="E75" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F74" s="2">
+      <c r="F75" s="2">
         <v>24</v>
-      </c>
-      <c r="G74" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B75" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F75" s="2">
-        <v>18</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>8</v>
@@ -2262,16 +2265,16 @@
         <v>5</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F76" s="2">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>8</v>
@@ -2282,100 +2285,100 @@
         <v>5</v>
       </c>
       <c r="C77" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F77" s="2">
+        <v>8</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B78" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E77" s="2" t="s">
+      <c r="E78" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F77" s="2">
+      <c r="F78" s="2">
         <v>2.5</v>
       </c>
-      <c r="G77" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A78" s="3"/>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
-      <c r="G78" s="3"/>
+      <c r="G78" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A79" s="2" t="s">
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A80" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C80" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="D80" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="E80" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F79" s="2">
+      <c r="F80" s="2">
         <v>6</v>
       </c>
-      <c r="G79" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A80" s="3"/>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
-      <c r="G80" s="3"/>
+      <c r="G80" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A81" s="2" t="s">
+      <c r="A81" s="3"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A82" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B81" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C81" s="2" t="s">
+      <c r="B82" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D81" s="2" t="s">
+      <c r="D82" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="E82" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F81" s="2">
+      <c r="F82" s="2">
         <v>68</v>
-      </c>
-      <c r="G81" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B82" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F82" s="2">
-        <v>36</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>8</v>
@@ -2386,16 +2389,16 @@
         <v>22</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="F83" s="2">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>8</v>
@@ -2406,16 +2409,16 @@
         <v>22</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F84" s="2">
-        <v>25.5</v>
+        <v>27</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>8</v>
@@ -2426,16 +2429,16 @@
         <v>22</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>134</v>
+        <v>16</v>
       </c>
       <c r="F85" s="2">
-        <v>21.5</v>
+        <v>25.5</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>8</v>
@@ -2446,28 +2449,43 @@
         <v>22</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>32</v>
+        <v>134</v>
       </c>
       <c r="F86" s="2">
-        <v>20.5</v>
+        <v>21.5</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>133</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B87" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D88" s="2" t="s">
+      <c r="C87" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F87" s="2">
+        <v>20.5</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D89" s="2" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>